<commit_message>
grouped and counted errors at Ytre-Vika and Valsneset
</commit_message>
<xml_diff>
--- a/stian/DataFromBazefield/totalErrorsBessakerAndSkomaker.xlsx
+++ b/stian/DataFromBazefield/totalErrorsBessakerAndSkomaker.xlsx
@@ -1,16 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10908"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mortenolsenosvik/Documents/NTNU/XAI Prsjektoppgave/project-thesis/stian/DataFromBazefield/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042BF043-0278-F040-B459-EB7F643C4F77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="500"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="19200" windowHeight="23540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
   <si>
     <t>42 Pitch control error</t>
   </si>
@@ -75,14 +87,23 @@
     <t>67 Overtemperature</t>
   </si>
   <si>
-    <t>Skomakerfjellet</t>
+    <t>Valsneset</t>
+  </si>
+  <si>
+    <t>222:1 Turbine reset (quit button)</t>
+  </si>
+  <si>
+    <t>70 Generator overtemperature</t>
+  </si>
+  <si>
+    <t>Ytre Vika</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -134,6 +155,29 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="40"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -157,12 +201,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -171,6 +218,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -495,21 +550,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="28" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="29" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="54.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" style="1" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="50">
+    <row r="1" spans="1:2" ht="52" x14ac:dyDescent="0.6">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -517,7 +572,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -525,7 +580,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -533,7 +588,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -541,7 +596,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -549,7 +604,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -557,7 +612,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -565,7 +620,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -573,7 +628,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +636,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -589,7 +644,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -597,7 +652,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -605,7 +660,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -613,7 +668,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -621,7 +676,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -629,7 +684,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -637,7 +692,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -645,13 +700,306 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="50">
+    <row r="19" spans="1:2" ht="52" x14ac:dyDescent="0.6">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="5">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="5">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="5">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="5">
+        <v>11773</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="52" x14ac:dyDescent="0.6">
+      <c r="A39" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="5">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B51" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B56" s="5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" s="5">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:B17">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
     <sortCondition descending="1" ref="B1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>